<commit_message>
added the fucking comments
</commit_message>
<xml_diff>
--- a/static/output.xlsx
+++ b/static/output.xlsx
@@ -25,6 +25,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -62,7 +65,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="1" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="1">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="1" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="2">
+    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="1" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="164">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -394,7 +397,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -409,13 +412,31 @@
       <c r="B1" s="1">
         <v>1</v>
       </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" ht="14.214749999999999" customHeight="true">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>2.92</v>
+        <v>44.01</v>
+      </c>
+      <c r="C2" s="2">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2">
+        <v>34</v>
       </c>
     </row>
     <row r="3" ht="14.214749999999999" customHeight="true">
@@ -423,7 +444,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>2.96</v>
+        <v>50</v>
+      </c>
+      <c r="C3" s="2">
+        <v>48</v>
+      </c>
+      <c r="D3" s="2">
+        <v>51</v>
+      </c>
+      <c r="E3" s="2">
+        <v>43</v>
       </c>
     </row>
     <row r="4" ht="14.214749999999999" customHeight="true">
@@ -431,7 +461,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>2.86</v>
+        <v>32</v>
+      </c>
+      <c r="C4" s="2">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2">
+        <v>22</v>
       </c>
     </row>
     <row r="5" ht="14.214749999999999" customHeight="true">
@@ -439,7 +478,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>3.04</v>
+        <v>52</v>
+      </c>
+      <c r="C5" s="2">
+        <v>55</v>
+      </c>
+      <c r="D5" s="2">
+        <v>56</v>
+      </c>
+      <c r="E5" s="2">
+        <v>44</v>
       </c>
     </row>
     <row r="6" ht="14.214749999999999" customHeight="true">
@@ -447,7 +495,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>3.07</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="2">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2">
+        <v>26</v>
       </c>
     </row>
     <row r="7" ht="14.214749999999999" customHeight="true">
@@ -455,7 +512,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>2.85</v>
+        <v>36</v>
+      </c>
+      <c r="C7" s="2">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2">
+        <v>35</v>
+      </c>
+      <c r="E7" s="2">
+        <v>31</v>
       </c>
     </row>
     <row r="8" ht="14.214749999999999" customHeight="true">
@@ -463,7 +529,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>3</v>
+        <v>21</v>
+      </c>
+      <c r="C8" s="2">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2">
+        <v>21</v>
       </c>
     </row>
     <row r="9" ht="14.214749999999999" customHeight="true">
@@ -471,7 +546,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>2.92</v>
+        <v>29</v>
+      </c>
+      <c r="C9" s="2">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2">
+        <v>23</v>
+      </c>
+      <c r="E9" s="2">
+        <v>22</v>
       </c>
     </row>
     <row r="10" ht="14.214749999999999" customHeight="true">
@@ -479,7 +563,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>2.97</v>
+        <v>26</v>
+      </c>
+      <c r="C10" s="2">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2">
+        <v>44</v>
+      </c>
+      <c r="E10" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="11" ht="14.214749999999999" customHeight="true">
@@ -487,7 +580,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>2.97</v>
+        <v>24</v>
+      </c>
+      <c r="C11" s="2">
+        <v>22</v>
+      </c>
+      <c r="D11" s="2">
+        <v>22</v>
+      </c>
+      <c r="E11" s="2">
+        <v>44</v>
       </c>
     </row>
     <row r="12" ht="14.214749999999999" customHeight="true">
@@ -495,7 +597,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>3.09</v>
+        <v>18</v>
+      </c>
+      <c r="C12" s="2">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2">
+        <v>49</v>
       </c>
     </row>
     <row r="13" ht="14.214749999999999" customHeight="true">
@@ -503,7 +614,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>3.07</v>
+        <v>24</v>
+      </c>
+      <c r="C13" s="2">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2">
+        <v>26</v>
+      </c>
+      <c r="E13" s="2">
+        <v>23</v>
       </c>
     </row>
     <row r="14" ht="14.214749999999999" customHeight="true">
@@ -511,7 +631,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>2.99</v>
+        <v>19</v>
+      </c>
+      <c r="C14" s="2">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2">
+        <v>28</v>
       </c>
     </row>
     <row r="15" ht="14.214749999999999" customHeight="true">
@@ -519,7 +648,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>3.06</v>
+        <v>8</v>
+      </c>
+      <c r="C15" s="2">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2">
+        <v>12</v>
       </c>
     </row>
     <row r="16" ht="14.214749999999999" customHeight="true">
@@ -527,7 +665,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>3.05</v>
+        <v>24</v>
+      </c>
+      <c r="C16" s="2">
+        <v>18.1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>27</v>
+      </c>
+      <c r="E16" s="2">
+        <v>24</v>
       </c>
     </row>
     <row r="17" ht="14.214749999999999" customHeight="true">
@@ -535,7 +682,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>3.02</v>
+        <v>56</v>
+      </c>
+      <c r="C17" s="2">
+        <v>52</v>
+      </c>
+      <c r="D17" s="2">
+        <v>56</v>
+      </c>
+      <c r="E17" s="2">
+        <v>50</v>
       </c>
     </row>
     <row r="18" ht="14.214749999999999" customHeight="true">
@@ -543,7 +699,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>3.07</v>
+        <v>32.01</v>
+      </c>
+      <c r="C18" s="2">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2">
+        <v>18</v>
+      </c>
+      <c r="E18" s="2">
+        <v>25</v>
       </c>
     </row>
     <row r="19" ht="14.214749999999999" customHeight="true">
@@ -551,7 +716,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>2.91</v>
+        <v>8</v>
+      </c>
+      <c r="C19" s="2">
+        <v>12.01</v>
+      </c>
+      <c r="D19" s="2">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2">
+        <v>17</v>
       </c>
     </row>
     <row r="20" ht="14.214749999999999" customHeight="true">
@@ -559,7 +733,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>3.07</v>
+        <v>51</v>
+      </c>
+      <c r="C20" s="2">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2">
+        <v>52.01</v>
+      </c>
+      <c r="E20" s="2">
+        <v>49</v>
       </c>
     </row>
     <row r="21" ht="14.214749999999999" customHeight="true">
@@ -567,7 +750,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>3.2</v>
+        <v>30</v>
+      </c>
+      <c r="C21" s="2">
+        <v>28</v>
+      </c>
+      <c r="D21" s="2">
+        <v>35</v>
+      </c>
+      <c r="E21" s="2">
+        <v>22.01</v>
       </c>
     </row>
     <row r="22" ht="14.214749999999999" customHeight="true"/>

</xml_diff>